<commit_message>
Se agrega sección de busqueda en CMS, se cambian iconos de edición y se comienza a armar la estructura de la base de datos
</commit_message>
<xml_diff>
--- a/Distribuidores.xlsx
+++ b/Distribuidores.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\Web_Andez\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E440009-F136-4045-903E-04957DC731C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD60FD2-CCBF-43AE-8B75-E0AF231A3D05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B9E18CE2-01C8-4CDD-A94D-456C5801D768}"/>
   </bookViews>

</xml_diff>

<commit_message>
Se agrega icono informativo en CMS Catálogo y se agregan iconos de atributos.
</commit_message>
<xml_diff>
--- a/Distribuidores.xlsx
+++ b/Distribuidores.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20417"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\Web_Andez\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\02-PLANTA\14- POST VENTA\Web_Andez-master\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFD60FD2-CCBF-43AE-8B75-E0AF231A3D05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{285C1C37-3CD2-4483-89D1-DA850C6CDFC8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B9E18CE2-01C8-4CDD-A94D-456C5801D768}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="13500" windowHeight="6384" xr2:uid="{B9E18CE2-01C8-4CDD-A94D-456C5801D768}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -20,23 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="312" uniqueCount="242">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="273">
   <si>
     <t>ID</t>
   </si>
@@ -762,13 +751,106 @@
   </si>
   <si>
     <t>-62.25087</t>
+  </si>
+  <si>
+    <t>https://interiorescasilda.com.ar/</t>
+  </si>
+  <si>
+    <t>https://www.merlinosrl.com.ar/</t>
+  </si>
+  <si>
+    <t>https://www.masferreterias.com/</t>
+  </si>
+  <si>
+    <t>http://mosaicoschajari.com.ar/</t>
+  </si>
+  <si>
+    <t>https://marmolerialenzi.com.ar/</t>
+  </si>
+  <si>
+    <t>https://neostone.com.ar/</t>
+  </si>
+  <si>
+    <t>https://www.nimat.com.ar/</t>
+  </si>
+  <si>
+    <t>https://materialesnuevacasa.com.ar/</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/quboambientes/</t>
+  </si>
+  <si>
+    <t>https://tiendarevestir.com.ar/</t>
+  </si>
+  <si>
+    <t>https://www.sagosa.com.ar/</t>
+  </si>
+  <si>
+    <t>https://www.sakurasa.com/index.php</t>
+  </si>
+  <si>
+    <t>http://www.todosanitarios.com.ar/index.html</t>
+  </si>
+  <si>
+    <t>https://www.instagram.com/mundovsdeco/</t>
+  </si>
+  <si>
+    <t>Telefono</t>
+  </si>
+  <si>
+    <t>341-5284950/59</t>
+  </si>
+  <si>
+    <t>341-5284970</t>
+  </si>
+  <si>
+    <t>381-3662112</t>
+  </si>
+  <si>
+    <t>3865-422424</t>
+  </si>
+  <si>
+    <t>381-4321616</t>
+  </si>
+  <si>
+    <t>381-4218691</t>
+  </si>
+  <si>
+    <t>4016-2400</t>
+  </si>
+  <si>
+    <t>4772-4800</t>
+  </si>
+  <si>
+    <t>4717-3300</t>
+  </si>
+  <si>
+    <t>348-4436190</t>
+  </si>
+  <si>
+    <t>230-4474051</t>
+  </si>
+  <si>
+    <t>341-4522080</t>
+  </si>
+  <si>
+    <t>341-2653870</t>
+  </si>
+  <si>
+    <t>2148-8817</t>
+  </si>
+  <si>
+    <t>4255-7465</t>
+  </si>
+  <si>
+    <t>223-4107000</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -778,14 +860,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -808,17 +882,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hipervínculo" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1151,23 +1226,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{33FC27F4-3308-47B9-AAF9-C81C8F2520C9}">
-  <dimension ref="A1:H67"/>
+  <dimension ref="A1:I67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="68.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="21.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.5546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="35.109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="68.69921875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.69921875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="20.59765625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="35.09765625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1177,23 +1253,26 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" t="s">
+        <v>256</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>131</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>145</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1203,20 +1282,23 @@
       <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="D2" t="s">
+        <v>257</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="F2" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1226,20 +1308,23 @@
       <c r="C3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="D3" t="s">
+        <v>258</v>
+      </c>
+      <c r="E3" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>132</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1249,20 +1334,23 @@
       <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="D4" t="s">
+        <v>262</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="F4" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="G4" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1272,20 +1360,23 @@
       <c r="C5" t="s">
         <v>140</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="D5" t="s">
+        <v>261</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="F5" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>139</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1295,20 +1386,23 @@
       <c r="C6" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="1" t="s">
+      <c r="D6" t="s">
+        <v>260</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="E6" s="1" t="s">
+      <c r="F6" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>139</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1318,20 +1412,23 @@
       <c r="C7" t="s">
         <v>155</v>
       </c>
-      <c r="D7" s="1" t="s">
+      <c r="D7" t="s">
+        <v>259</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E7" s="1" t="s">
+      <c r="F7" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
         <v>139</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1341,20 +1438,23 @@
       <c r="C8" t="s">
         <v>14</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="3" t="s">
+        <v>266</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="F8" s="2" t="s">
+      <c r="G8" s="2" t="s">
         <v>161</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1364,20 +1464,23 @@
       <c r="C9" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="D9" t="s">
+        <v>263</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="E9" s="1" t="s">
+      <c r="F9" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="F9" t="s">
+      <c r="G9" t="s">
         <v>161</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1387,20 +1490,23 @@
       <c r="C10" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="D10" t="s">
+        <v>265</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="E10" s="1" t="s">
+      <c r="F10" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="F10" t="s">
+      <c r="G10" t="s">
         <v>161</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1410,20 +1516,23 @@
       <c r="C11" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="1" t="s">
+      <c r="D11" t="s">
+        <v>264</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="E11" s="1" t="s">
+      <c r="F11" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>161</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1433,20 +1542,23 @@
       <c r="C12" t="s">
         <v>22</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" t="s">
+        <v>267</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="F12" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="F12" t="s">
+      <c r="G12" t="s">
         <v>161</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1457,7 +1569,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1468,7 +1580,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1478,20 +1590,23 @@
       <c r="C15" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="1" t="s">
+      <c r="D15" t="s">
+        <v>268</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="E15" s="1" t="s">
+      <c r="F15" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="F15" s="2" t="s">
+      <c r="G15" s="2" t="s">
         <v>177</v>
       </c>
-      <c r="G15" t="s">
+      <c r="H15" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1501,20 +1616,23 @@
       <c r="C16" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="F16" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="F16" t="s">
+      <c r="G16" t="s">
         <v>177</v>
       </c>
-      <c r="G16" t="s">
+      <c r="H16" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1524,20 +1642,23 @@
       <c r="C17" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" t="s">
+        <v>270</v>
+      </c>
+      <c r="E17" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="F17" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="F17" s="2" t="s">
+      <c r="G17" s="2" t="s">
         <v>182</v>
       </c>
-      <c r="G17" t="s">
+      <c r="H17" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1547,20 +1668,23 @@
       <c r="C18" t="s">
         <v>183</v>
       </c>
-      <c r="D18" s="1" t="s">
+      <c r="D18" t="s">
+        <v>271</v>
+      </c>
+      <c r="E18" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="E18" s="1" t="s">
+      <c r="F18" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="F18" t="s">
+      <c r="G18" t="s">
         <v>182</v>
       </c>
-      <c r="G18" t="s">
+      <c r="H18" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1570,20 +1694,23 @@
       <c r="C19" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" t="s">
+        <v>272</v>
+      </c>
+      <c r="E19" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="F19" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="F19" s="2" t="s">
+      <c r="G19" s="2" t="s">
         <v>186</v>
       </c>
-      <c r="G19" t="s">
+      <c r="H19" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1593,20 +1720,23 @@
       <c r="C20" t="s">
         <v>187</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" t="s">
+        <v>272</v>
+      </c>
+      <c r="E20" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="F20" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="F20" t="s">
+      <c r="G20" t="s">
         <v>186</v>
       </c>
-      <c r="G20" t="s">
+      <c r="H20" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1616,20 +1746,20 @@
       <c r="C21" t="s">
         <v>38</v>
       </c>
-      <c r="D21" s="1" t="s">
+      <c r="E21" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="E21" s="1" t="s">
+      <c r="F21" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="F21" s="2" t="s">
+      <c r="G21" s="2" t="s">
         <v>194</v>
       </c>
-      <c r="G21" t="s">
+      <c r="H21" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1639,20 +1769,20 @@
       <c r="C22" t="s">
         <v>40</v>
       </c>
-      <c r="D22" s="1" t="s">
+      <c r="E22" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="E22" s="1" t="s">
+      <c r="F22" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="F22" s="2" t="s">
+      <c r="G22" s="2" t="s">
         <v>195</v>
       </c>
-      <c r="G22" t="s">
+      <c r="H22" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1662,20 +1792,20 @@
       <c r="C23" t="s">
         <v>42</v>
       </c>
-      <c r="D23" s="1" t="s">
+      <c r="E23" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="E23" s="1" t="s">
+      <c r="F23" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="F23" s="2" t="s">
+      <c r="G23" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="G23" t="s">
+      <c r="H23" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1685,20 +1815,20 @@
       <c r="C24" t="s">
         <v>200</v>
       </c>
-      <c r="D24" s="1" t="s">
+      <c r="E24" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="E24" s="1" t="s">
+      <c r="F24" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
         <v>198</v>
       </c>
-      <c r="G24" t="s">
+      <c r="H24" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1708,20 +1838,20 @@
       <c r="C25" t="s">
         <v>45</v>
       </c>
-      <c r="D25" s="1" t="s">
+      <c r="E25" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="E25" s="1" t="s">
+      <c r="F25" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="F25" s="2" t="s">
+      <c r="G25" s="2" t="s">
         <v>205</v>
       </c>
-      <c r="G25" t="s">
+      <c r="H25" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1731,20 +1861,20 @@
       <c r="C26" t="s">
         <v>47</v>
       </c>
-      <c r="D26" s="1" t="s">
+      <c r="E26" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="E26" s="1" t="s">
+      <c r="F26" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="F26" s="2" t="s">
+      <c r="G26" s="2" t="s">
         <v>207</v>
       </c>
-      <c r="G26" t="s">
+      <c r="H26" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1754,20 +1884,20 @@
       <c r="C27" t="s">
         <v>49</v>
       </c>
-      <c r="D27" s="1" t="s">
+      <c r="E27" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="E27" s="1" t="s">
+      <c r="F27" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="F27" t="s">
+      <c r="G27" t="s">
         <v>207</v>
       </c>
-      <c r="G27" t="s">
+      <c r="H27" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1777,20 +1907,20 @@
       <c r="C28" t="s">
         <v>51</v>
       </c>
-      <c r="D28" s="1" t="s">
+      <c r="E28" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="E28" s="1" t="s">
+      <c r="F28" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="F28" t="s">
+      <c r="G28" t="s">
         <v>207</v>
       </c>
-      <c r="G28" t="s">
+      <c r="H28" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:8">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1800,20 +1930,20 @@
       <c r="C29" t="s">
         <v>53</v>
       </c>
-      <c r="D29" s="1" t="s">
+      <c r="E29" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="E29" s="1" t="s">
+      <c r="F29" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="F29" t="s">
+      <c r="G29" t="s">
         <v>174</v>
       </c>
-      <c r="G29" t="s">
+      <c r="H29" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:8">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1823,20 +1953,20 @@
       <c r="C30" t="s">
         <v>55</v>
       </c>
-      <c r="D30" s="1" t="s">
+      <c r="E30" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="E30" s="1" t="s">
+      <c r="F30" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="F30" t="s">
+      <c r="G30" t="s">
         <v>212</v>
       </c>
-      <c r="G30" t="s">
+      <c r="H30" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:8">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1846,20 +1976,20 @@
       <c r="C31" t="s">
         <v>57</v>
       </c>
-      <c r="D31" s="1" t="s">
+      <c r="E31" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="E31" s="1" t="s">
+      <c r="F31" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="F31" t="s">
+      <c r="G31" t="s">
         <v>215</v>
       </c>
-      <c r="G31" t="s">
+      <c r="H31" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:8">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1869,20 +1999,20 @@
       <c r="C32" t="s">
         <v>59</v>
       </c>
-      <c r="D32" s="1" t="s">
+      <c r="E32" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="E32" s="1" t="s">
+      <c r="F32" s="1" t="s">
         <v>220</v>
       </c>
-      <c r="F32" t="s">
+      <c r="G32" t="s">
         <v>218</v>
       </c>
-      <c r="G32" t="s">
+      <c r="H32" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:8">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1892,20 +2022,20 @@
       <c r="C33" t="s">
         <v>61</v>
       </c>
-      <c r="D33" s="1" t="s">
+      <c r="E33" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="E33" s="1" t="s">
+      <c r="F33" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="F33" t="s">
+      <c r="G33" t="s">
         <v>221</v>
       </c>
-      <c r="G33" t="s">
+      <c r="H33" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:8">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1915,20 +2045,20 @@
       <c r="C34" t="s">
         <v>62</v>
       </c>
-      <c r="D34" s="1" t="s">
+      <c r="E34" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="E34" s="1" t="s">
+      <c r="F34" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="F34" t="s">
+      <c r="G34" t="s">
         <v>221</v>
       </c>
-      <c r="G34" t="s">
+      <c r="H34" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:8">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1938,20 +2068,20 @@
       <c r="C35" t="s">
         <v>64</v>
       </c>
-      <c r="D35" s="1" t="s">
+      <c r="E35" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="E35" s="1" t="s">
+      <c r="F35" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="F35" t="s">
+      <c r="G35" t="s">
         <v>226</v>
       </c>
-      <c r="G35" t="s">
+      <c r="H35" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:8">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1961,20 +2091,20 @@
       <c r="C36" t="s">
         <v>66</v>
       </c>
-      <c r="D36" s="1" t="s">
+      <c r="E36" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="E36" s="1" t="s">
+      <c r="F36" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="F36" t="s">
+      <c r="G36" t="s">
         <v>229</v>
       </c>
-      <c r="G36" t="s">
+      <c r="H36" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:8">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1984,20 +2114,20 @@
       <c r="C37" t="s">
         <v>68</v>
       </c>
-      <c r="D37" s="1" t="s">
+      <c r="E37" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="E37" s="1" t="s">
+      <c r="F37" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="F37" t="s">
+      <c r="G37" t="s">
         <v>229</v>
       </c>
-      <c r="G37" t="s">
+      <c r="H37" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:8">
       <c r="A38">
         <v>37</v>
       </c>
@@ -2007,20 +2137,20 @@
       <c r="C38" t="s">
         <v>70</v>
       </c>
-      <c r="D38" s="1" t="s">
+      <c r="E38" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="E38" s="1" t="s">
+      <c r="F38" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="F38" t="s">
+      <c r="G38" t="s">
         <v>236</v>
       </c>
-      <c r="G38" t="s">
+      <c r="H38" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:8">
       <c r="A39">
         <v>38</v>
       </c>
@@ -2030,14 +2160,14 @@
       <c r="C39" t="s">
         <v>72</v>
       </c>
-      <c r="F39" t="s">
+      <c r="G39" t="s">
         <v>237</v>
       </c>
-      <c r="G39" t="s">
+      <c r="H39" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:8">
       <c r="A40">
         <v>39</v>
       </c>
@@ -2047,14 +2177,14 @@
       <c r="C40" t="s">
         <v>74</v>
       </c>
-      <c r="F40" t="s">
+      <c r="G40" t="s">
         <v>237</v>
       </c>
-      <c r="G40" t="s">
+      <c r="H40" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:8">
       <c r="A41">
         <v>40</v>
       </c>
@@ -2064,14 +2194,14 @@
       <c r="C41" t="s">
         <v>115</v>
       </c>
-      <c r="F41" t="s">
+      <c r="G41" t="s">
         <v>237</v>
       </c>
-      <c r="G41" t="s">
+      <c r="H41" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:8">
       <c r="A42">
         <v>41</v>
       </c>
@@ -2081,14 +2211,14 @@
       <c r="C42" t="s">
         <v>116</v>
       </c>
-      <c r="F42" t="s">
+      <c r="G42" t="s">
         <v>237</v>
       </c>
-      <c r="G42" t="s">
+      <c r="H42" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:8">
       <c r="A43">
         <v>42</v>
       </c>
@@ -2099,10 +2229,13 @@
         <v>78</v>
       </c>
       <c r="G43" t="s">
+        <v>242</v>
+      </c>
+      <c r="H43" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:8">
       <c r="A44">
         <v>43</v>
       </c>
@@ -2113,10 +2246,13 @@
         <v>80</v>
       </c>
       <c r="G44" t="s">
+        <v>243</v>
+      </c>
+      <c r="H44" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:8">
       <c r="A45">
         <v>44</v>
       </c>
@@ -2127,10 +2263,13 @@
         <v>82</v>
       </c>
       <c r="G45" t="s">
+        <v>243</v>
+      </c>
+      <c r="H45" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:8">
       <c r="A46">
         <v>45</v>
       </c>
@@ -2141,10 +2280,13 @@
         <v>84</v>
       </c>
       <c r="G46" t="s">
+        <v>243</v>
+      </c>
+      <c r="H46" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:8">
       <c r="A47">
         <v>46</v>
       </c>
@@ -2155,10 +2297,13 @@
         <v>86</v>
       </c>
       <c r="G47" t="s">
+        <v>243</v>
+      </c>
+      <c r="H47" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:8">
       <c r="A48">
         <v>47</v>
       </c>
@@ -2169,10 +2314,13 @@
         <v>88</v>
       </c>
       <c r="G48" t="s">
+        <v>244</v>
+      </c>
+      <c r="H48" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:8">
       <c r="A49">
         <v>48</v>
       </c>
@@ -2183,10 +2331,13 @@
         <v>90</v>
       </c>
       <c r="G49" t="s">
+        <v>245</v>
+      </c>
+      <c r="H49" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:8">
       <c r="A50">
         <v>49</v>
       </c>
@@ -2197,10 +2348,13 @@
         <v>93</v>
       </c>
       <c r="G50" t="s">
+        <v>246</v>
+      </c>
+      <c r="H50" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:8">
       <c r="A51">
         <v>50</v>
       </c>
@@ -2211,10 +2365,13 @@
         <v>94</v>
       </c>
       <c r="G51" t="s">
+        <v>246</v>
+      </c>
+      <c r="H51" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:8">
       <c r="A52">
         <v>51</v>
       </c>
@@ -2225,10 +2382,13 @@
         <v>96</v>
       </c>
       <c r="G52" t="s">
+        <v>246</v>
+      </c>
+      <c r="H52" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:8">
       <c r="A53">
         <v>52</v>
       </c>
@@ -2239,10 +2399,13 @@
         <v>98</v>
       </c>
       <c r="G53" t="s">
+        <v>247</v>
+      </c>
+      <c r="H53" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:8">
       <c r="A54">
         <v>53</v>
       </c>
@@ -2253,10 +2416,13 @@
         <v>100</v>
       </c>
       <c r="G54" t="s">
+        <v>248</v>
+      </c>
+      <c r="H54" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:8">
       <c r="A55">
         <v>54</v>
       </c>
@@ -2267,10 +2433,13 @@
         <v>102</v>
       </c>
       <c r="G55" t="s">
+        <v>249</v>
+      </c>
+      <c r="H55" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:8">
       <c r="A56">
         <v>55</v>
       </c>
@@ -2281,10 +2450,13 @@
         <v>104</v>
       </c>
       <c r="G56" t="s">
+        <v>249</v>
+      </c>
+      <c r="H56" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:8">
       <c r="A57">
         <v>56</v>
       </c>
@@ -2295,10 +2467,13 @@
         <v>106</v>
       </c>
       <c r="G57" t="s">
+        <v>249</v>
+      </c>
+      <c r="H57" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:8">
       <c r="A58">
         <v>57</v>
       </c>
@@ -2308,11 +2483,14 @@
       <c r="C58" t="s">
         <v>108</v>
       </c>
-      <c r="G58" t="s">
+      <c r="G58" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="H58" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:8">
       <c r="A59">
         <v>58</v>
       </c>
@@ -2323,10 +2501,13 @@
         <v>110</v>
       </c>
       <c r="G59" t="s">
+        <v>251</v>
+      </c>
+      <c r="H59" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:8">
       <c r="A60">
         <v>59</v>
       </c>
@@ -2337,10 +2518,13 @@
         <v>112</v>
       </c>
       <c r="G60" t="s">
+        <v>252</v>
+      </c>
+      <c r="H60" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:8">
       <c r="A61">
         <v>60</v>
       </c>
@@ -2351,10 +2535,13 @@
         <v>114</v>
       </c>
       <c r="G61" t="s">
+        <v>253</v>
+      </c>
+      <c r="H61" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="62" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:8">
       <c r="A62">
         <v>61</v>
       </c>
@@ -2365,10 +2552,13 @@
         <v>118</v>
       </c>
       <c r="G62" t="s">
+        <v>253</v>
+      </c>
+      <c r="H62" t="s">
         <v>239</v>
       </c>
     </row>
-    <row r="63" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:8">
       <c r="A63">
         <v>62</v>
       </c>
@@ -2379,10 +2569,13 @@
         <v>121</v>
       </c>
       <c r="G63" t="s">
+        <v>253</v>
+      </c>
+      <c r="H63" t="s">
         <v>240</v>
       </c>
     </row>
-    <row r="64" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:8">
       <c r="A64">
         <v>63</v>
       </c>
@@ -2393,10 +2586,13 @@
         <v>122</v>
       </c>
       <c r="G64" t="s">
+        <v>253</v>
+      </c>
+      <c r="H64" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:8">
       <c r="A65">
         <v>64</v>
       </c>
@@ -2407,10 +2603,13 @@
         <v>124</v>
       </c>
       <c r="G65" t="s">
+        <v>254</v>
+      </c>
+      <c r="H65" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:8">
       <c r="A66">
         <v>65</v>
       </c>
@@ -2420,11 +2619,14 @@
       <c r="C66" t="s">
         <v>127</v>
       </c>
-      <c r="G66" t="s">
+      <c r="G66" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="H66" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:8">
       <c r="A67">
         <v>66</v>
       </c>
@@ -2434,23 +2636,13 @@
       <c r="C67" t="s">
         <v>128</v>
       </c>
+      <c r="G67" s="2" t="s">
+        <v>255</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1" xr:uid="{66A86699-E365-459A-96FC-F0C2908E4099}"/>
-    <hyperlink ref="F4" r:id="rId2" xr:uid="{A0D94422-155D-4D88-95BF-F8A0A574A79A}"/>
-    <hyperlink ref="F8" r:id="rId3" xr:uid="{020925A7-26C0-4773-8165-66A65B040EA2}"/>
-    <hyperlink ref="F15" r:id="rId4" xr:uid="{F8BD34E5-B393-45CA-ABF6-BFE150A679A5}"/>
-    <hyperlink ref="F17" r:id="rId5" xr:uid="{B9B7F867-066C-4C08-9843-883284DA5350}"/>
-    <hyperlink ref="F19" r:id="rId6" xr:uid="{A5DA61A8-3FF9-4F20-9FE2-5B391B2C092C}"/>
-    <hyperlink ref="F21" r:id="rId7" xr:uid="{D08FACEB-0D6A-4F09-A33F-A6391A0029FE}"/>
-    <hyperlink ref="F22" r:id="rId8" xr:uid="{3FF41014-AA12-4D9D-B98B-8F4240258500}"/>
-    <hyperlink ref="F23" r:id="rId9" xr:uid="{3BDDFF19-2E14-45BA-A048-419B96144FE0}"/>
-    <hyperlink ref="F25" r:id="rId10" xr:uid="{5ABB6089-05EE-4450-A0E2-A71025ACFA41}"/>
-    <hyperlink ref="F26" r:id="rId11" xr:uid="{C5161C38-C09D-48EA-9025-5F7D2CF9DC4F}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId12"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>